<commit_message>
finished initial testing of the APIs, included a spreadsheet denoting which ones work and which ones don't
</commit_message>
<xml_diff>
--- a/api_function_complete_tracker.xlsx
+++ b/api_function_complete_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buy003/Documents/GitHub/galah_python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4F22A1-C27D-DF45-AF3A-4C0929B595EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429D6E15-0811-ED42-8CDC-B715913ED46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16860" yWindow="1580" windowWidth="31760" windowHeight="18740" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
+    <workbookView xWindow="500" yWindow="1140" windowWidth="31760" windowHeight="18740" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="63">
   <si>
     <t>Australia</t>
   </si>
@@ -203,23 +203,35 @@
     <t>Reasons</t>
   </si>
   <si>
-    <t>fix or debug</t>
-  </si>
-  <si>
-    <t>unsure - probably depends</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>Network</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Not working</t>
+  </si>
+  <si>
+    <t>Returns empty</t>
+  </si>
+  <si>
+    <t>unsure what to do - see comment in box</t>
+  </si>
+  <si>
+    <t>fix or debug; includes network errors</t>
+  </si>
+  <si>
+    <t>done/error handled</t>
+  </si>
+  <si>
+    <t>Canada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -230,6 +242,13 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -288,13 +307,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC5FAE6-11E8-4F4F-8869-11F223FB8C9D}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -624,7 +644,7 @@
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -727,11 +747,15 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="M3" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="N3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="3"/>
+      <c r="O3" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="P3" s="4" t="s">
         <v>51</v>
       </c>
@@ -753,29 +777,29 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="M4" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="N4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="2"/>
+      <c r="O4" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="P4" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -783,105 +807,125 @@
       <c r="J5" s="2"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="2"/>
+      <c r="M5" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="N5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O5" s="2"/>
+      <c r="O5" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="P5" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="2"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="N6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O6" s="2"/>
+      <c r="O6" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="P6" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="N7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="O7" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="P7" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
       <c r="J8" s="2"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="2"/>
+      <c r="M8" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="N8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O8" s="2"/>
+      <c r="O8" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="P8" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -889,56 +933,62 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" s="2"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="N9" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O9" s="2"/>
+      <c r="O9" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="P9" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="N10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O10" s="2"/>
+      <c r="O10" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="P10" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="3"/>
@@ -947,292 +997,411 @@
       <c r="J11" s="2"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="2"/>
+      <c r="M11" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="N11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="O11" s="2"/>
+      <c r="O11" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="P11" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>39</v>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="H15" s="5"/>
       <c r="I15" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H16" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="H16" s="4"/>
       <c r="I16" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="3"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
       <c r="L22" s="4"/>
-      <c r="M22" s="2"/>
+      <c r="M22" s="3"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="3"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="2"/>
+      <c r="M23" s="3"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" s="3"/>
       <c r="L24" s="4"/>
-      <c r="M24" s="2"/>
+      <c r="M24" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>3</v>
+      <c r="A25" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K25" s="3"/>
       <c r="L25" s="4"/>
-      <c r="M25" s="2"/>
+      <c r="M25" s="3"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K26" s="3"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="2"/>
+      <c r="M26" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>58</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K27" s="3"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="2"/>
+      <c r="M27" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>58</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28" s="3"/>
       <c r="L28" s="4"/>
-      <c r="M28" s="2"/>
+      <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="3"/>
+      <c r="E29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="L29" s="4"/>
-      <c r="M29" s="5"/>
+      <c r="M29" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="K30" s="3"/>
       <c r="L30" s="4"/>
       <c r="M30" s="3"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K31" s="3"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="3"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K32" s="3"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed some bugs; added the Spanish and Brazilian Atlas; still need to get occurrences working
</commit_message>
<xml_diff>
--- a/api_function_complete_tracker.xlsx
+++ b/api_function_complete_tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buy003/Documents/GitHub/galah_python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buy003/Documents/GitHub/galah-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429D6E15-0811-ED42-8CDC-B715913ED46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F20556-1DFA-7044-8B51-5B9015374D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="1140" windowWidth="31760" windowHeight="18740" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
+    <workbookView xWindow="11360" yWindow="1100" windowWidth="35020" windowHeight="18120" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="58">
   <si>
     <t>Australia</t>
   </si>
@@ -116,24 +116,12 @@
     <t>show_values</t>
   </si>
   <si>
-    <t>X*</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>**</t>
   </si>
   <si>
-    <t>***</t>
-  </si>
-  <si>
-    <t>****</t>
-  </si>
-  <si>
-    <t>*****</t>
-  </si>
-  <si>
     <t xml:space="preserve">***** </t>
   </si>
   <si>
@@ -191,9 +179,6 @@
     <t>Profiles</t>
   </si>
   <si>
-    <t>IP</t>
-  </si>
-  <si>
     <t>Providers</t>
   </si>
   <si>
@@ -203,18 +188,9 @@
     <t>Reasons</t>
   </si>
   <si>
-    <t>Network</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
-    <t>Not working</t>
-  </si>
-  <si>
-    <t>Returns empty</t>
-  </si>
-  <si>
     <t>unsure what to do - see comment in box</t>
   </si>
   <si>
@@ -225,13 +201,23 @@
   </si>
   <si>
     <t>Canada</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Unsure what to do</t>
+  </si>
+  <si>
+    <t>unable to verify
+user details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -249,6 +235,14 @@
     <font>
       <sz val="16"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -307,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -315,6 +309,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -333,7 +332,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -621,7 +620,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -632,7 +631,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -642,7 +641,7 @@
     <col min="3" max="3" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -714,8 +713,8 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
+      <c r="F2" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -733,409 +732,339 @@
         <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" ht="44" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="E4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="F5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="F8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" ht="44" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="E10" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="F11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="F12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>51</v>
-      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1152,32 +1081,30 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="4"/>
+      <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="B23" s="2"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="3"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K23" s="2"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="2"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="3"/>
@@ -1186,222 +1113,186 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="4" t="s">
-        <v>58</v>
+      <c r="H24" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="K24" s="3"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="B25" s="2"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="3"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K25" s="2"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="6" t="s">
-        <v>56</v>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K26" s="2"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K27" s="3"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="6" t="s">
-        <v>56</v>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" s="2"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="2"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K28" s="3"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="3"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="2"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="B29" s="2"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I29" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L29" s="4"/>
-      <c r="M29" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="2"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
       <c r="K30" s="3"/>
-      <c r="L30" s="4"/>
+      <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="3"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I31" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K31" s="3"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="3"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="2"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="2"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="3"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K32" s="2"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added integration tests for Brazilian atlas, fixed up tests for Australian atlas
</commit_message>
<xml_diff>
--- a/api_function_complete_tracker.xlsx
+++ b/api_function_complete_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buy003/Documents/GitHub/galah-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F20556-1DFA-7044-8B51-5B9015374D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6521EF39-D7D9-524A-8805-2469009E1BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11360" yWindow="1100" windowWidth="35020" windowHeight="18120" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
+    <workbookView xWindow="9720" yWindow="1720" windowWidth="35020" windowHeight="18120" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t>Australia</t>
   </si>
@@ -98,9 +98,6 @@
     <t>search_taxa</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Austria**</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
   </si>
   <si>
     <t>Austria</t>
-  </si>
-  <si>
-    <t>Unsure what to do</t>
   </si>
   <si>
     <t>unable to verify
@@ -631,7 +625,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -641,7 +635,7 @@
     <col min="3" max="3" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -691,31 +685,27 @@
         <v>19</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F2" s="4"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -729,17 +719,15 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F3" s="4"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -751,21 +739,17 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:16" ht="44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -779,17 +763,15 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -806,14 +788,12 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F6" s="4"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -830,14 +810,12 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F7" s="4"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -854,14 +832,12 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F8" s="4"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -878,14 +854,12 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F9" s="4"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -902,16 +876,14 @@
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="2"/>
       <c r="E10" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="F10" s="4"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -928,14 +900,12 @@
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -952,14 +922,12 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F12" s="4"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -973,98 +941,98 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1086,7 +1054,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
@@ -1097,7 +1065,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="3"/>
@@ -1114,11 +1082,11 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -1126,7 +1094,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
@@ -1135,13 +1103,13 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="3"/>
@@ -1159,15 +1127,15 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="3"/>
       <c r="M26" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1181,18 +1149,18 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="3"/>
       <c r="M27" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1207,10 +1175,10 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="3"/>
@@ -1228,10 +1196,10 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="3"/>
@@ -1266,10 +1234,10 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="3"/>
@@ -1288,7 +1256,7 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="3"/>

</xml_diff>

<commit_message>
adding other atlases, refactoring code etc.
</commit_message>
<xml_diff>
--- a/api_function_complete_tracker.xlsx
+++ b/api_function_complete_tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buy003/Documents/GitHub/galah-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6521EF39-D7D9-524A-8805-2469009E1BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4AD03A-1201-6544-822B-48C8575D4C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="1720" windowWidth="35020" windowHeight="18120" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
+    <workbookView xWindow="53160" yWindow="9020" windowWidth="35020" windowHeight="18120" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
   <si>
     <t>Australia</t>
   </si>
@@ -98,9 +98,6 @@
     <t>search_taxa</t>
   </si>
   <si>
-    <t>Austria**</t>
-  </si>
-  <si>
     <t>search_all</t>
   </si>
   <si>
@@ -203,15 +200,23 @@
     <t>Austria</t>
   </si>
   <si>
-    <t>unable to verify
-user details</t>
+    <t>GBIF</t>
+  </si>
+  <si>
+    <t>Order of addition:</t>
+  </si>
+  <si>
+    <t>not working</t>
+  </si>
+  <si>
+    <t>later</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -235,6 +240,23 @@
     </font>
     <font>
       <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -295,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -305,9 +327,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC5FAE6-11E8-4F4F-8869-11F223FB8C9D}">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M9" sqref="M9:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -644,7 +666,7 @@
     <col min="12" max="12" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.83203125" style="1"/>
-    <col min="15" max="15" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -685,27 +707,27 @@
         <v>19</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -718,38 +740,42 @@
       <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
+      <c r="A3" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -763,15 +789,17 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -788,12 +816,14 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -806,60 +836,74 @@
       <c r="P6" s="2"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -871,63 +915,67 @@
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="44" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="4"/>
+      <c r="F12" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -939,141 +987,161 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>34</v>
-      </c>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="1" t="s">
-        <v>51</v>
+        <v>33</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="H16" s="5"/>
       <c r="I16" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P16" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="H18" s="3"/>
+      <c r="I18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M21" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K23" s="2"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M23" s="3"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1082,42 +1150,40 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="2"/>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K25" s="2"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="3"/>
+      <c r="J25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
@@ -1125,22 +1191,22 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
+      <c r="H26" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="I26" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
@@ -1148,104 +1214,114 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="8" t="s">
-        <v>49</v>
-      </c>
+      <c r="H27" s="2"/>
       <c r="I27" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="3"/>
       <c r="M27" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="2"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K28" s="2"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="L28" s="3"/>
-      <c r="M28" s="2"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="2"/>
+      <c r="M28" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K29" s="2"/>
+      <c r="E29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="2"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M29" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="B30" s="2"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="2"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M30" s="2"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K31" s="2"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="2"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>8</v>
+      <c r="M31" s="3"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>
@@ -1254,13 +1330,51 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
+      <c r="I32" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="J32" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="3"/>
       <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K33" s="2"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added Austrian and French atlases.  Fixed up atlas_species for atlases already integrated into galah.  Added lots of integration tests.
</commit_message>
<xml_diff>
--- a/api_function_complete_tracker.xlsx
+++ b/api_function_complete_tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buy003/Documents/GitHub/galah-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4AD03A-1201-6544-822B-48C8575D4C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FF3A08-C0C7-7542-B7D5-25075D2B63AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53160" yWindow="9020" windowWidth="35020" windowHeight="18120" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34000" windowHeight="18480" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="59">
   <si>
     <t>Australia</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>later</t>
+  </si>
+  <si>
+    <t>Sweden**</t>
   </si>
 </sst>
 </file>
@@ -647,7 +650,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9:P9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -664,7 +667,7 @@
     <col min="10" max="10" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.83203125" style="1"/>
     <col min="15" max="15" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -797,9 +800,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -821,9 +822,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -842,18 +841,18 @@
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -898,22 +897,34 @@
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="C9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="F9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -925,9 +936,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -970,22 +979,34 @@
       <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="F12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -997,9 +1018,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1037,7 +1056,7 @@
         <v>50</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1052,7 +1071,7 @@
         <v>49</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1065,9 +1084,6 @@
       <c r="H18" s="3"/>
       <c r="I18" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -1285,79 +1301,91 @@
       <c r="A30" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K30" s="2"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="2"/>
+      <c r="M30" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="3"/>
+      <c r="B31" s="2"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31" s="2"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
+      <c r="M31" s="2"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K32" s="2"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K32" s="3"/>
       <c r="L32" s="3"/>
-      <c r="M32" s="2"/>
+      <c r="M32" s="3"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="2"/>
+      <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K33" s="2"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K33" s="3"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="2"/>
+      <c r="M33" s="6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">

</xml_diff>

<commit_message>
fixed atlas_species so it returns a list of all taxa specified by what rank you want
</commit_message>
<xml_diff>
--- a/api_function_complete_tracker.xlsx
+++ b/api_function_complete_tracker.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buy003/Documents/GitHub/galah-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FF3A08-C0C7-7542-B7D5-25075D2B63AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81D491A-9FA8-D249-B450-D635623B7C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34000" windowHeight="18480" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
+    <workbookView xWindow="25260" yWindow="760" windowWidth="25340" windowHeight="20020" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="names for taxa" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="86">
   <si>
     <t>Australia</t>
   </si>
@@ -213,6 +214,87 @@
   </si>
   <si>
     <t>Sweden**</t>
+  </si>
+  <si>
+    <t>Guatemala**</t>
+  </si>
+  <si>
+    <t>Kingdom</t>
+  </si>
+  <si>
+    <t>Phylum</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Genus</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Subspecies</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>kingdom, kingdomID</t>
+  </si>
+  <si>
+    <t>phylum, phylumID</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>genus</t>
+  </si>
+  <si>
+    <t>class, classID</t>
+  </si>
+  <si>
+    <t>kingdom</t>
+  </si>
+  <si>
+    <t>phylum</t>
+  </si>
+  <si>
+    <t>species, species_guid</t>
+  </si>
+  <si>
+    <t>subspecies_guid, subspecies_name</t>
+  </si>
+  <si>
+    <t>subspecies, subspeciesID</t>
+  </si>
+  <si>
+    <t>species, speciesID</t>
+  </si>
+  <si>
+    <t>kingdom, kingdom_id</t>
+  </si>
+  <si>
+    <t>phylum, phylum_id</t>
+  </si>
+  <si>
+    <t>subspecies,subspecies_guid, subspecies_name</t>
   </si>
 </sst>
 </file>
@@ -650,7 +732,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1138,7 @@
         <v>50</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1407,4 +1489,308 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A7BAA53-E587-3148-A5AE-55CA5C76824C}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="52.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed GBIF APIs so atlas_occurrences will authenticate correctly
</commit_message>
<xml_diff>
--- a/api_function_complete_tracker.xlsx
+++ b/api_function_complete_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buy003/Documents/GitHub/galah-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81D491A-9FA8-D249-B450-D635623B7C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BCCB0F-7201-7045-9952-4914C0217944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25260" yWindow="760" windowWidth="25340" windowHeight="20020" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
+    <workbookView xWindow="55540" yWindow="5600" windowWidth="28800" windowHeight="15540" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="87">
   <si>
     <t>Australia</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>subspecies,subspecies_guid, subspecies_name</t>
+  </si>
+  <si>
+    <t>Not supported</t>
   </si>
 </sst>
 </file>
@@ -732,7 +735,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -746,7 +749,7 @@
     <col min="7" max="7" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14" style="1" bestFit="1" customWidth="1"/>
@@ -951,17 +954,15 @@
       <c r="D8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
         <v>56</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="4" t="s">
-        <v>56</v>
+      <c r="J8" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>

</xml_diff>

<commit_message>
fixed arguments in atlas_occurrences to include all, working on GBIF, Guatemala and Spanish atlases
</commit_message>
<xml_diff>
--- a/api_function_complete_tracker.xlsx
+++ b/api_function_complete_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buy003/Documents/GitHub/galah-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BCCB0F-7201-7045-9952-4914C0217944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD24052-709C-9144-A875-660079708DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55540" yWindow="5600" windowWidth="28800" windowHeight="15540" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
+    <workbookView xWindow="0" yWindow="7460" windowWidth="38400" windowHeight="19360" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="87">
   <si>
     <t>Australia</t>
   </si>
@@ -735,7 +735,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -966,9 +966,7 @@
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>

</xml_diff>

<commit_message>
adding more commits before release
</commit_message>
<xml_diff>
--- a/api_function_complete_tracker.xlsx
+++ b/api_function_complete_tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buy003/Documents/GitHub/galah-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716F7612-110E-4043-A568-24D3E02CFBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECA9568-53B3-6440-8C4B-399F90323DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34980" windowHeight="17100" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
   </bookViews>
@@ -738,7 +738,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -824,6 +824,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
+      <c r="I2" s="2"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -848,6 +849,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -872,6 +874,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -894,6 +897,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -916,6 +920,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -940,6 +945,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
+      <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -964,6 +970,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
+      <c r="I8" s="2"/>
       <c r="J8" s="3"/>
       <c r="K8" s="6" t="s">
         <v>86</v>
@@ -998,6 +1005,7 @@
       <c r="H9" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="I9" s="2"/>
       <c r="J9" s="4" t="s">
         <v>56</v>
       </c>
@@ -1024,6 +1032,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1048,6 +1057,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
+      <c r="I11" s="2"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -1080,6 +1090,7 @@
       <c r="H12" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="I12" s="2"/>
       <c r="J12" s="4" t="s">
         <v>56</v>
       </c>
@@ -1106,6 +1117,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>

</xml_diff>

<commit_message>
refactor(adding-build-files-and-api-tracker): adding build files and api tracker
</commit_message>
<xml_diff>
--- a/api_function_complete_tracker.xlsx
+++ b/api_function_complete_tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buy003/Documents/GitHub/galah-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECA9568-53B3-6440-8C4B-399F90323DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F9CFEF-6A2C-8F46-92F5-423E390D79F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34980" windowHeight="17100" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="34980" windowHeight="17100" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -737,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC5FAE6-11E8-4F4F-8869-11F223FB8C9D}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -824,7 +824,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="2"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>

</xml_diff>

<commit_message>
feat(added-guatemalan-and-swedish-atlases): added guatemalan and swedish atlases
</commit_message>
<xml_diff>
--- a/api_function_complete_tracker.xlsx
+++ b/api_function_complete_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buy003/Documents/GitHub/galah-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F9CFEF-6A2C-8F46-92F5-423E390D79F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD5E785-0295-D644-9964-75A2C590ECAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="34980" windowHeight="17100" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34980" windowHeight="17100" xr2:uid="{2654DB72-6E78-694F-B5AD-C86B11E46023}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="85">
   <si>
     <t>Australia</t>
   </si>
@@ -204,19 +204,10 @@
     <t>GBIF</t>
   </si>
   <si>
-    <t>Order of addition:</t>
-  </si>
-  <si>
     <t>not working</t>
   </si>
   <si>
     <t>later</t>
-  </si>
-  <si>
-    <t>Sweden**</t>
-  </si>
-  <si>
-    <t>Guatemala**</t>
   </si>
   <si>
     <t>Kingdom</t>
@@ -439,9 +430,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -479,7 +470,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -585,7 +576,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -727,7 +718,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -737,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC5FAE6-11E8-4F4F-8869-11F223FB8C9D}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -786,7 +777,7 @@
         <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>17</v>
@@ -843,7 +834,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -868,7 +859,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -939,7 +930,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -964,7 +955,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -973,7 +964,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="3"/>
       <c r="K8" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -989,29 +980,19 @@
       <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="H9" s="3"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -1051,7 +1032,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1074,29 +1055,19 @@
       <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="H12" s="3"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -1134,12 +1105,7 @@
       <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="O15" s="10"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1152,11 +1118,8 @@
       <c r="I16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1167,11 +1130,8 @@
       <c r="I17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1183,7 +1143,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
@@ -1191,12 +1151,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
         <v>36</v>
@@ -1235,7 +1195,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>0</v>
       </c>
@@ -1252,7 +1212,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>53</v>
       </c>
@@ -1273,7 +1233,7 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>1</v>
       </c>
@@ -1294,7 +1254,7 @@
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
@@ -1317,7 +1277,7 @@
       <c r="L26" s="3"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
@@ -1340,7 +1300,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>3</v>
       </c>
@@ -1367,7 +1327,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>54</v>
       </c>
@@ -1394,7 +1354,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>4</v>
       </c>
@@ -1419,7 +1379,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>5</v>
       </c>
@@ -1440,7 +1400,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="2"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>6</v>
       </c>
@@ -1529,28 +1489,28 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1558,28 +1518,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1587,28 +1547,28 @@
         <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1616,28 +1576,28 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1671,28 +1631,28 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="H7" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1755,28 +1715,28 @@
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="H11" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>